<commit_message>
Firm v0.8 - update
</commit_message>
<xml_diff>
--- a/Firmware/v0.8 - Hard v0.4 - Beta/LCD - EEPROM - Layout - Firm v08.xlsx
+++ b/Firmware/v0.8 - Hard v0.4 - Beta/LCD - EEPROM - Layout - Firm v08.xlsx
@@ -745,8 +745,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AF83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="R83" sqref="R83"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="L83" sqref="L83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3891,25 +3891,25 @@
         <v>19</v>
       </c>
       <c r="O81" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P81" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q81" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R81" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="S81" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="P81" s="1" t="s">
+      <c r="T81" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="Q81" s="6" t="s">
+      <c r="U81" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="R81" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="S81" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="T81" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="U81" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="V81" s="6"/>
       <c r="Y81" s="6"/>
@@ -4054,8 +4054,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:EE33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="DZ30" sqref="DZ30"/>
+    <sheetView topLeftCell="CQ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Firm v0.8 - Hard v0.4
</commit_message>
<xml_diff>
--- a/Firmware/v0.8 - Hard v0.4 - Beta/LCD - EEPROM - Layout - Firm v08.xlsx
+++ b/Firmware/v0.8 - Hard v0.4 - Beta/LCD - EEPROM - Layout - Firm v08.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="86">
   <si>
     <t>01</t>
   </si>
@@ -743,10 +743,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:AF83"/>
+  <dimension ref="A1:AF95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="L83" sqref="L83"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="U59" sqref="U59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2480,214 +2480,71 @@
       <c r="U49" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V49" s="6"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M50" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N50" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O50" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P50" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q50" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T50" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="U50" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V50" s="6"/>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="5"/>
       <c r="D51" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O51" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G51" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L51" s="5"/>
-      <c r="M51" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N51" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="P51" s="1" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="V51" s="6"/>
+        <v>56</v>
+      </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L52" s="5"/>
-      <c r="M52" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O52" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q52" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R52" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S52" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T52" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U52" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="V52" s="6"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L53" s="5"/>
-      <c r="M53" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N53" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O53" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P53" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q53" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R53" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="S53" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T53" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="V53" s="6"/>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
@@ -2756,237 +2613,75 @@
       <c r="A56" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J56" s="5"/>
-      <c r="K56" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O56" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P56" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q56" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S56" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T56" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U56" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O57" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J57" s="5"/>
-      <c r="K57" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L57" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M57" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O57" s="5"/>
-      <c r="P57" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q57" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="R57" s="6" t="s">
-        <v>45</v>
+      <c r="P57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R57" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="S57" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="T57" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B58" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J58" s="5"/>
-      <c r="K58" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O58" s="5"/>
-      <c r="P58" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q58" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="R58" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="S58" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T58" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U58" s="1" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J59" s="5"/>
-      <c r="K59" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L59" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M59" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O59" s="5"/>
-      <c r="P59" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q59" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="R59" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="S59" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T59" s="1" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="P60" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q60" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R60" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S60" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U60" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A60" s="7"/>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
@@ -3050,6 +2745,7 @@
       <c r="U61" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="V61" s="6"/>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
@@ -3059,186 +2755,206 @@
         <v>21</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E62" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P62" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K62" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L62" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="Q62" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T62" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U62" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V62" s="6"/>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E63" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H63" s="6" t="s">
+      <c r="C63" s="5"/>
+      <c r="D63" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I63" s="6" t="s">
+      <c r="I63" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J63" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J63" s="5"/>
-      <c r="K63" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L63" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M63" s="6" t="s">
-        <v>19</v>
+      <c r="L63" s="5"/>
+      <c r="M63" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="P63" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="Q63" s="1" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="R63" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S63" s="1" t="s">
-        <v>59</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="V63" s="6"/>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C64" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D64" s="6" t="s">
+      <c r="C64" s="5"/>
+      <c r="D64" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H64" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="I64" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L64" s="5"/>
+      <c r="M64" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P64" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q64" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R64" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S64" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T64" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U64" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J64" s="5"/>
-      <c r="K64" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L64" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M64" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P64" s="5"/>
-      <c r="Q64" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="R64" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="S64" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="T64" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="V64" s="6"/>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="C65" s="5"/>
       <c r="D65" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L65" s="5"/>
+      <c r="M65" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N65" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O65" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P65" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q65" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E65" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G65" s="6" t="s">
+      <c r="R65" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S65" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H65" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I65" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J65" s="5"/>
-      <c r="K65" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L65" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M65" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P65" s="5"/>
-      <c r="Q65" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="R65" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="S65" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="T65" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U65" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="V65" s="6"/>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="2" t="s">
         <v>53</v>
@@ -3301,169 +3017,243 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>64</v>
+        <v>26</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J68" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="J68" s="5"/>
       <c r="K68" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P68" s="5"/>
-      <c r="Q68" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="R68" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="S68" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T68" s="6" t="s">
-        <v>52</v>
+        <v>19</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O68" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P68" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S68" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T68" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="U68" s="1" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E69" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J69" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="B69" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J69" s="5"/>
       <c r="K69" s="6" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="L69" s="6" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="M69" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N69" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O69" s="5"/>
+      <c r="P69" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q69" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O69" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="R69" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="S69" s="6" t="s">
-        <v>19</v>
+        <v>45</v>
+      </c>
+      <c r="S69" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B70" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="G70" s="1" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="H70" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J70" s="5"/>
+      <c r="K70" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O70" s="5"/>
+      <c r="P70" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q70" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="R70" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S70" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I70" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K70" s="1" t="s">
+      <c r="T70" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L70" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M70" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N70" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O70" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P70" s="5"/>
-      <c r="Q70" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R70" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="S70" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="T70" s="6"/>
+      <c r="U70" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I71" s="6"/>
-      <c r="J71" s="6"/>
-      <c r="K71" s="6"/>
-      <c r="L71" s="6"/>
-      <c r="M71" s="6"/>
-      <c r="P71" s="5"/>
-      <c r="Q71" s="6" t="s">
+      <c r="B71" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J71" s="5"/>
+      <c r="K71" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L71" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M71" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O71" s="5"/>
+      <c r="P71" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q71" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R71" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S71" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T71" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="P72" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R71" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="S71" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="T71" s="6" t="s">
+      <c r="Q72" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R72" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="S72" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T72" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U72" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="2" t="s">
         <v>53</v>
@@ -3526,220 +3316,194 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F74" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="G74" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N74" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="O74" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="P74" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q74" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R74" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="T74" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D75" s="6" t="s">
+      <c r="E75" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H75" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E75" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G75" s="6" t="s">
+      <c r="I75" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J75" s="5"/>
+      <c r="K75" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L75" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M75" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N75" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O75" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I75" s="5"/>
-      <c r="J75" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="K75" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L75" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M75" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N75" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P75" s="5"/>
-      <c r="Q75" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="R75" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="S75" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="T75" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="U75" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE75" s="1"/>
-      <c r="AF75" s="1"/>
+      <c r="P75" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q75" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R75" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S75" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B76" s="5"/>
       <c r="C76" s="6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I76" s="5"/>
-      <c r="J76" s="6" t="s">
-        <v>65</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J76" s="5"/>
       <c r="K76" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L76" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="M76" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N76" s="1" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="P76" s="5"/>
       <c r="Q76" s="6" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="R76" s="6" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="S76" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="T76" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="U76" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE76" s="1"/>
-      <c r="AF76" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="T76" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>23</v>
+      <c r="C77" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I77" s="5"/>
-      <c r="J77" s="6" t="s">
-        <v>65</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I77" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J77" s="5"/>
       <c r="K77" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L77" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M77" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P77" s="5"/>
+      <c r="Q77" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="R77" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S77" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L77" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M77" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N77" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P77" s="6"/>
-      <c r="Q77" s="6"/>
-      <c r="R77" s="6"/>
-      <c r="S77" s="6"/>
-      <c r="T77" s="6"/>
-      <c r="AE77" s="1"/>
-      <c r="AF77" s="1"/>
+      <c r="T77" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U77" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="2" t="s">
         <v>53</v>
@@ -3801,101 +3565,93 @@
       <c r="U79" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V79" s="6"/>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="E80" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P80" s="5"/>
+      <c r="Q80" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R80" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="S80" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T80" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J80" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L80" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M80" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N80" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O80" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="P80" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q80" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S80" s="6"/>
-      <c r="T80" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="U80" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V80" s="6"/>
+        <v>44</v>
+      </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="E81" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="F81" s="6" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I81" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J81" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K81" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="J81" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K81" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="L81" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M81" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N81" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O81" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P81" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="M81" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N81" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O81" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P81" s="5"/>
       <c r="Q81" s="6" t="s">
         <v>19</v>
       </c>
@@ -3903,145 +3659,659 @@
         <v>19</v>
       </c>
       <c r="S81" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="T81" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="U81" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="V81" s="6"/>
-      <c r="Y81" s="6"/>
-      <c r="Z81" s="6"/>
-      <c r="AA81" s="6"/>
-      <c r="AB81" s="6"/>
-      <c r="AC81" s="6"/>
+        <v>19</v>
+      </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B82" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G82" s="1" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>24</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K82" s="5"/>
-      <c r="L82" s="6" t="s">
-        <v>19</v>
+        <v>44</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L82" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>19</v>
+        <v>44</v>
+      </c>
+      <c r="O82" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="P82" s="5"/>
       <c r="Q82" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R82" s="6" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="S82" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="T82" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V82" s="6"/>
-      <c r="Y82" s="6"/>
-      <c r="Z82" s="6"/>
-      <c r="AA82" s="6"/>
-      <c r="AB82" s="6"/>
-      <c r="AC82" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="T82" s="6"/>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G83" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K83" s="5"/>
-      <c r="L83" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M83" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N83" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="6"/>
       <c r="P83" s="5"/>
       <c r="Q83" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="R83" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S83" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="T83" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="85" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+      <c r="B85" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J85" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L85" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M85" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N85" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O85" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P85" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q85" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R85" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S85" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T85" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U85" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L86" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M86" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O86" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="P86" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q86" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R86" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="S86" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U86" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" s="5"/>
+      <c r="C87" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I87" s="5"/>
+      <c r="J87" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K87" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L87" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M87" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="N87" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P87" s="5"/>
+      <c r="Q87" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="R87" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S87" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T87" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="U87" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE87" s="1"/>
+      <c r="AF87" s="1"/>
+    </row>
+    <row r="88" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B88" s="5"/>
+      <c r="C88" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I88" s="5"/>
+      <c r="J88" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K88" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L88" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M88" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="N88" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P88" s="5"/>
+      <c r="Q88" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="R88" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S88" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T88" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="U88" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE88" s="1"/>
+      <c r="AF88" s="1"/>
+    </row>
+    <row r="89" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="5"/>
+      <c r="C89" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I89" s="5"/>
+      <c r="J89" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K89" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L89" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M89" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="N89" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P89" s="5"/>
+      <c r="Q89" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R89" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S89" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="T89" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE89" s="1"/>
+      <c r="AF89" s="1"/>
+    </row>
+    <row r="91" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+      <c r="B91" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J91" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K91" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M91" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N91" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O91" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P91" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q91" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R91" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S91" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T91" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U91" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V91" s="6"/>
+    </row>
+    <row r="92" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="R83" s="1" t="s">
+      <c r="C92" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L92" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N92" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O92" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="P92" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q92" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S92" s="6"/>
+      <c r="T92" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="U92" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V92" s="6"/>
+    </row>
+    <row r="93" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I93" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K93" s="5"/>
+      <c r="L93" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N93" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O93" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P93" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q93" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R93" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="S93" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="T93" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="U93" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="V93" s="6"/>
+      <c r="Y93" s="6"/>
+      <c r="Z93" s="6"/>
+      <c r="AA93" s="6"/>
+      <c r="AB93" s="6"/>
+      <c r="AC93" s="6"/>
+    </row>
+    <row r="94" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F94" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S83" s="1" t="s">
+      <c r="G94" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H94" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="T83" s="1" t="s">
+      <c r="I94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K94" s="5"/>
+      <c r="L94" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M94" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N94" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P94" s="5"/>
+      <c r="Q94" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="R94" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S94" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="U83" s="1" t="s">
+      <c r="T94" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V94" s="6"/>
+      <c r="Y94" s="6"/>
+      <c r="Z94" s="6"/>
+      <c r="AA94" s="6"/>
+      <c r="AB94" s="6"/>
+      <c r="AC94" s="1"/>
+    </row>
+    <row r="95" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G95" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K95" s="5"/>
+      <c r="L95" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P95" s="5"/>
+      <c r="Q95" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="R95" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="V83" s="6"/>
-      <c r="Y83" s="6"/>
-      <c r="Z83" s="6"/>
-      <c r="AA83" s="6"/>
-      <c r="AB83" s="6"/>
-      <c r="AC83" s="1"/>
+      <c r="S95" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T95" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U95" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V95" s="6"/>
+      <c r="Y95" s="6"/>
+      <c r="Z95" s="6"/>
+      <c r="AA95" s="6"/>
+      <c r="AB95" s="6"/>
+      <c r="AC95" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>